<commit_message>
Update Site Cluster IWIP SSU005
</commit_message>
<xml_diff>
--- a/data/datek-cluster-iwip.xlsx
+++ b/data/datek-cluster-iwip.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4BCA9E-873A-439D-A1C2-1582330F5315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87B30E7-6366-4F7B-A28C-28649FB2CEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,9 +171,6 @@
     <t>mz19900215</t>
   </si>
   <si>
-    <t>Maret@2025</t>
-  </si>
-  <si>
     <t>SSU043</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>SBM</t>
+  </si>
+  <si>
+    <t>Juni@2025</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -723,7 +723,7 @@
         <v>45</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -743,7 +743,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>41</v>
@@ -758,7 +758,7 @@
         <v>42</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -778,7 +778,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>41</v>
@@ -793,7 +793,7 @@
         <v>42</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -813,7 +813,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>41</v>
@@ -848,7 +848,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>41</v>
@@ -883,7 +883,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>41</v>
@@ -918,7 +918,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>41</v>
@@ -930,10 +930,10 @@
         <v>25</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -953,7 +953,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>41</v>
@@ -965,10 +965,10 @@
         <v>27</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>

</xml_diff>

<commit_message>
Seperate Monitor Donggala to Main Segment & Detail Segment
</commit_message>
<xml_diff>
--- a/data/datek-cluster-iwip.xlsx
+++ b/data/datek-cluster-iwip.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87B30E7-6366-4F7B-A28C-28649FB2CEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B5C1AB-BA5C-4283-8273-CD9ECE1B7287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
   <si>
     <t>Hostname NE</t>
   </si>
@@ -67,12 +67,6 @@
   </si>
   <si>
     <t>10.199.238.199</t>
-  </si>
-  <si>
-    <t>SW-D7-SFI-SSU005-NEW</t>
-  </si>
-  <si>
-    <t>172.25.106.15</t>
   </si>
   <si>
     <t>SW-D7-SFI-SSU043</t>
@@ -165,12 +159,6 @@
     <t>Telkom123!</t>
   </si>
   <si>
-    <t>SSU005</t>
-  </si>
-  <si>
-    <t>mz19900215</t>
-  </si>
-  <si>
     <t>SSU043</t>
   </si>
   <si>
@@ -196,9 +184,6 @@
   </si>
   <si>
     <t>SBM</t>
-  </si>
-  <si>
-    <t>Juni@2025</t>
   </si>
 </sst>
 </file>
@@ -478,11 +463,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:U1001"/>
+  <dimension ref="A1:U1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -496,10 +481,10 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -508,13 +493,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -533,10 +518,10 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -545,10 +530,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -568,10 +553,10 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
@@ -580,10 +565,10 @@
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -603,10 +588,10 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -615,10 +600,10 @@
         <v>7</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -638,10 +623,10 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>8</v>
@@ -650,10 +635,10 @@
         <v>9</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -673,10 +658,10 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>10</v>
@@ -685,10 +670,10 @@
         <v>11</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -708,10 +693,10 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>12</v>
@@ -720,10 +705,10 @@
         <v>13</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -743,10 +728,10 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>14</v>
@@ -755,10 +740,10 @@
         <v>15</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -778,10 +763,10 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>16</v>
@@ -790,10 +775,10 @@
         <v>17</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -813,10 +798,10 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>18</v>
@@ -825,10 +810,10 @@
         <v>19</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -848,10 +833,10 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>20</v>
@@ -860,10 +845,10 @@
         <v>21</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -883,10 +868,10 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>22</v>
@@ -895,10 +880,10 @@
         <v>23</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -918,10 +903,10 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>24</v>
@@ -930,10 +915,10 @@
         <v>25</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -952,24 +937,12 @@
       <c r="U13" s="3"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -1264,7 +1237,7 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-      <c r="B27" s="4"/>
+      <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
@@ -1451,8 +1424,8 @@
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
@@ -23664,29 +23637,6 @@
       <c r="T1000" s="3"/>
       <c r="U1000" s="3"/>
     </row>
-    <row r="1001" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1001" s="3"/>
-      <c r="B1001" s="3"/>
-      <c r="C1001" s="3"/>
-      <c r="D1001" s="3"/>
-      <c r="E1001" s="3"/>
-      <c r="F1001" s="3"/>
-      <c r="G1001" s="3"/>
-      <c r="H1001" s="3"/>
-      <c r="I1001" s="3"/>
-      <c r="J1001" s="3"/>
-      <c r="K1001" s="3"/>
-      <c r="L1001" s="3"/>
-      <c r="M1001" s="3"/>
-      <c r="N1001" s="3"/>
-      <c r="O1001" s="3"/>
-      <c r="P1001" s="3"/>
-      <c r="Q1001" s="3"/>
-      <c r="R1001" s="3"/>
-      <c r="S1001" s="3"/>
-      <c r="T1001" s="3"/>
-      <c r="U1001" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>